<commit_message>
NC: Added Vendor and TR, Updated add rows (MODIFY & VIEW not yet)
</commit_message>
<xml_diff>
--- a/ExpenseProcessingSystem/ExpenseProcessingSystem/wwwroot/ExcelTemplates/_ReportLayout_12.xlsx
+++ b/ExpenseProcessingSystem/ExpenseProcessingSystem/wwwroot/ExcelTemplates/_ReportLayout_12.xlsx
@@ -5,14 +5,14 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\akio.fujiwara\Desktop\EXPRESS project\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Work\Mizuho EPS\eps_source\ExpenseProcessingSystem\ExpenseProcessingSystem\wwwroot\ExcelTemplates\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="-24120" yWindow="-1590" windowWidth="24240" windowHeight="13140"/>
   </bookViews>
   <sheets>
-    <sheet name="TransactionList" sheetId="1" r:id="rId1"/>
+    <sheet name="Prepaid Amort Schedule" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -29,10 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
-  <si>
-    <t>Voucher Number</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="15">
   <si>
     <t>Check Number</t>
   </si>
@@ -49,59 +46,41 @@
     <t>Remarks</t>
   </si>
   <si>
-    <t>Debit/Credit</t>
-  </si>
-  <si>
-    <t>Currency</t>
-  </si>
-  <si>
     <t>Amount</t>
   </si>
   <si>
-    <t>Customer</t>
-  </si>
-  <si>
-    <t>Account Code</t>
-  </si>
-  <si>
-    <t>Account Number</t>
-  </si>
-  <si>
-    <t>Account Name</t>
-  </si>
-  <si>
-    <t>Exchange Rate</t>
-  </si>
-  <si>
-    <t>Contra Currency</t>
-  </si>
-  <si>
-    <t>Fund</t>
-  </si>
-  <si>
-    <t>Advice Print</t>
-  </si>
-  <si>
-    <t>Details</t>
-  </si>
-  <si>
-    <t>Entity</t>
-  </si>
-  <si>
-    <t>Division</t>
-  </si>
-  <si>
-    <t>Inter-Amount</t>
-  </si>
-  <si>
-    <t>Inter-Rate</t>
+    <t>Vendor</t>
+  </si>
+  <si>
+    <t>First Month of Amortization</t>
+  </si>
+  <si>
+    <t>Day</t>
+  </si>
+  <si>
+    <t>No. of Months</t>
+  </si>
+  <si>
+    <t>Schedule of Amortization</t>
+  </si>
+  <si>
+    <t>Name</t>
+  </si>
+  <si>
+    <t>TIN</t>
+  </si>
+  <si>
+    <t>Address</t>
+  </si>
+  <si>
+    <t>Prepaid Amortization Schedule Report</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -116,6 +95,27 @@
       <name val="Meiryo UI"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Meiryo UI"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -125,7 +125,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -133,14 +133,92 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -156,6 +234,55 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>256556</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>43644</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>1344706</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>189446</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="256556" y="43644"/>
+          <a:ext cx="1088150" cy="336302"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -455,18 +582,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:ED2"/>
+  <dimension ref="A1:ED14"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="J13" sqref="J13"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="20.5703125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="17.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="31" customWidth="1"/>
     <col min="4" max="4" width="17.140625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="9.5703125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="18" customWidth="1"/>
     <col min="7" max="7" width="19.85546875" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="15.7109375" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="14.5703125" bestFit="1" customWidth="1"/>
@@ -597,73 +726,55 @@
     <col min="134" max="134" width="17.5703125" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
+    <row r="1" spans="1:134" x14ac:dyDescent="0.25">
+      <c r="A1" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="B1" s="11"/>
+      <c r="C1" s="11"/>
+      <c r="D1" s="11"/>
+      <c r="E1" s="11"/>
+      <c r="F1" s="11"/>
+      <c r="G1" s="11"/>
+      <c r="H1" s="13"/>
+      <c r="I1" s="13"/>
+      <c r="J1" s="13"/>
+      <c r="K1" s="13"/>
+      <c r="L1" s="13"/>
+      <c r="M1" s="13"/>
+      <c r="N1" s="13"/>
+      <c r="O1" s="13"/>
+      <c r="P1" s="13"/>
+      <c r="Q1" s="13"/>
+      <c r="R1" s="13"/>
+      <c r="S1" s="13"/>
+      <c r="T1" s="13"/>
+      <c r="U1" s="13"/>
+      <c r="V1" s="13"/>
+    </row>
     <row r="2" spans="1:134" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="F2" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="G2" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="H2" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="I2" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="J2" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="K2" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="L2" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="M2" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="N2" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="O2" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="P2" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="Q2" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="R2" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="S2" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="T2" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="U2" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="V2" s="2" t="s">
-        <v>21</v>
-      </c>
+      <c r="A2" s="12"/>
+      <c r="B2" s="12"/>
+      <c r="C2" s="12"/>
+      <c r="D2" s="12"/>
+      <c r="E2" s="12"/>
+      <c r="F2" s="12"/>
+      <c r="G2" s="12"/>
+      <c r="H2" s="12"/>
+      <c r="I2" s="12"/>
+      <c r="J2" s="12"/>
+      <c r="K2" s="12"/>
+      <c r="L2" s="12"/>
+      <c r="M2" s="12"/>
+      <c r="N2" s="12"/>
+      <c r="O2" s="12"/>
+      <c r="P2" s="12"/>
+      <c r="Q2" s="12"/>
+      <c r="R2" s="12"/>
+      <c r="S2" s="12"/>
+      <c r="T2" s="12"/>
+      <c r="U2" s="12"/>
+      <c r="V2" s="12"/>
       <c r="W2" s="2"/>
       <c r="X2" s="2"/>
       <c r="Y2" s="2"/>
@@ -777,7 +888,191 @@
       <c r="EC2" s="2"/>
       <c r="ED2" s="2"/>
     </row>
+    <row r="3" spans="1:134" x14ac:dyDescent="0.25">
+      <c r="A3" s="17" t="s">
+        <v>11</v>
+      </c>
+      <c r="B3" s="12"/>
+      <c r="C3" s="12"/>
+      <c r="D3" s="12"/>
+      <c r="E3" s="12"/>
+      <c r="F3" s="14"/>
+      <c r="G3" s="14"/>
+      <c r="H3" s="14"/>
+      <c r="I3" s="14"/>
+      <c r="J3" s="14"/>
+      <c r="K3" s="14"/>
+      <c r="L3" s="14"/>
+      <c r="M3" s="14"/>
+      <c r="N3" s="14"/>
+      <c r="O3" s="14"/>
+      <c r="P3" s="14"/>
+      <c r="Q3" s="14"/>
+      <c r="R3" s="14"/>
+      <c r="S3" s="14"/>
+      <c r="T3" s="14"/>
+      <c r="U3" s="14"/>
+      <c r="V3" s="14"/>
+    </row>
+    <row r="4" spans="1:134" x14ac:dyDescent="0.25">
+      <c r="A4" s="17" t="s">
+        <v>12</v>
+      </c>
+      <c r="B4" s="12"/>
+      <c r="C4" s="12"/>
+      <c r="D4" s="12"/>
+      <c r="E4" s="12"/>
+      <c r="F4" s="14"/>
+      <c r="G4" s="14"/>
+      <c r="H4" s="14"/>
+      <c r="I4" s="14"/>
+      <c r="J4" s="14"/>
+      <c r="K4" s="14"/>
+      <c r="L4" s="14"/>
+      <c r="M4" s="14"/>
+      <c r="N4" s="14"/>
+      <c r="O4" s="14"/>
+      <c r="P4" s="14"/>
+      <c r="Q4" s="14"/>
+      <c r="R4" s="14"/>
+      <c r="S4" s="14"/>
+      <c r="T4" s="14"/>
+      <c r="U4" s="14"/>
+      <c r="V4" s="14"/>
+    </row>
+    <row r="5" spans="1:134" x14ac:dyDescent="0.25">
+      <c r="A5" s="17" t="s">
+        <v>13</v>
+      </c>
+      <c r="B5" s="12"/>
+      <c r="C5" s="12"/>
+      <c r="D5" s="12"/>
+      <c r="E5" s="12"/>
+      <c r="F5" s="14"/>
+      <c r="G5" s="14"/>
+      <c r="H5" s="14"/>
+      <c r="I5" s="14"/>
+      <c r="J5" s="14"/>
+      <c r="K5" s="14"/>
+      <c r="L5" s="14"/>
+      <c r="M5" s="14"/>
+      <c r="N5" s="14"/>
+      <c r="O5" s="14"/>
+      <c r="P5" s="14"/>
+      <c r="Q5" s="14"/>
+      <c r="R5" s="14"/>
+      <c r="S5" s="14"/>
+      <c r="T5" s="14"/>
+      <c r="U5" s="14"/>
+      <c r="V5" s="14"/>
+    </row>
+    <row r="6" spans="1:134" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B6" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="C6" s="4"/>
+      <c r="D6" s="5"/>
+      <c r="E6" s="5"/>
+      <c r="F6" s="5"/>
+      <c r="G6" s="5"/>
+    </row>
+    <row r="7" spans="1:134" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B7" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C7" s="4"/>
+      <c r="D7" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="E7" s="4"/>
+      <c r="F7" s="5"/>
+      <c r="G7" s="5"/>
+    </row>
+    <row r="8" spans="1:134" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B8" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C8" s="4"/>
+      <c r="D8" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="E8" s="10"/>
+      <c r="F8" s="9"/>
+      <c r="G8" s="9"/>
+    </row>
+    <row r="9" spans="1:134" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B9" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C9" s="4"/>
+      <c r="D9" s="2"/>
+      <c r="E9" s="5"/>
+      <c r="F9" s="5"/>
+      <c r="G9" s="5"/>
+    </row>
+    <row r="10" spans="1:134" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B10" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C10" s="4"/>
+      <c r="D10" s="5"/>
+      <c r="E10" s="5"/>
+      <c r="F10" s="5"/>
+      <c r="G10" s="5"/>
+    </row>
+    <row r="11" spans="1:134" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="B11" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C11" s="4"/>
+      <c r="D11" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E11" s="4"/>
+      <c r="F11" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="G11" s="4"/>
+    </row>
+    <row r="12" spans="1:134" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B12" s="6"/>
+      <c r="C12" s="5"/>
+      <c r="D12" s="5"/>
+      <c r="E12" s="5"/>
+      <c r="F12" s="5"/>
+      <c r="G12" s="5"/>
+    </row>
+    <row r="13" spans="1:134" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B13" s="15" t="s">
+        <v>10</v>
+      </c>
+      <c r="C13" s="16"/>
+      <c r="D13" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="E13" s="8"/>
+      <c r="F13" s="8"/>
+      <c r="G13" s="8"/>
+    </row>
+    <row r="14" spans="1:134" x14ac:dyDescent="0.25">
+      <c r="B14" s="1"/>
+      <c r="C14" s="1"/>
+      <c r="D14" s="1"/>
+      <c r="E14" s="1"/>
+      <c r="F14" s="1"/>
+      <c r="G14" s="1"/>
+    </row>
   </sheetData>
+  <mergeCells count="6">
+    <mergeCell ref="A1:G1"/>
+    <mergeCell ref="B3:E3"/>
+    <mergeCell ref="B4:E4"/>
+    <mergeCell ref="B5:E5"/>
+    <mergeCell ref="B13:C13"/>
+    <mergeCell ref="A2:V2"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>